<commit_message>
gpu thing, fixed questions, axed viewer
</commit_message>
<xml_diff>
--- a/data/manipulation_tasks.xlsx
+++ b/data/manipulation_tasks.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qtcc\OneDrive\Desktop\rvl\llm_rl_for_manipulation\vector-trl-references-main\examples\genesis-grpo\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qtcc\OneDrive\Desktop\rvl\llm_rl_for_manipulation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31751C85-14FB-48CA-9C71-26B08FB3AC2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C467BB0-1A8F-42A3-9ED7-32FA8DF139B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,15 +42,6 @@
     <t>green_cube_goal</t>
   </si>
   <si>
-    <t>(-0.25,0.25,0,0.02)</t>
-  </si>
-  <si>
-    <t>(0.25,0.5,0,0.02)</t>
-  </si>
-  <si>
-    <t>(-0.25,0.5,0,0.02)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Take the block with a colour on the Canadian flag, and move it to the position (0,0.375,0.02). </t>
   </si>
   <si>
@@ -60,13 +51,22 @@
     <t xml:space="preserve">Take the block that is the same colour as the ocean, and move it to the position (0,0.375,0.02). </t>
   </si>
   <si>
-    <t>(0.25,0.25,0,0.02)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Take the block that is the same colour as a traffic light that is telling cars to "go", and move it to the position (0,0.375,0.02). </t>
   </si>
   <si>
     <t xml:space="preserve">Take the block that is the colour of the Saharah Desert, and move it to the position (0,0.375,0.02). </t>
+  </si>
+  <si>
+    <t>(0.25,0.25,0.02)</t>
+  </si>
+  <si>
+    <t>(-0.25,0.25,0.02)</t>
+  </si>
+  <si>
+    <t>(0.25,0.5,0.02)</t>
+  </si>
+  <si>
+    <t>(-0.25,0.5,0.02)</t>
   </si>
 </sst>
 </file>
@@ -387,7 +387,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -418,70 +418,70 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>6</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
         <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed model, and data
</commit_message>
<xml_diff>
--- a/data/manipulation_tasks.xlsx
+++ b/data/manipulation_tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qtcc\OneDrive\Desktop\rvl\llm_rl_for_manipulation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C467BB0-1A8F-42A3-9ED7-32FA8DF139B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CDD5C49-E44D-434D-9E2C-3877B9859C54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Text Question</t>
   </si>
@@ -42,24 +42,9 @@
     <t>green_cube_goal</t>
   </si>
   <si>
-    <t xml:space="preserve">Take the block with a colour on the Canadian flag, and move it to the position (0,0.375,0.02). </t>
-  </si>
-  <si>
     <t>(0,0.375,0.02)</t>
   </si>
   <si>
-    <t xml:space="preserve">Take the block that is the same colour as the ocean, and move it to the position (0,0.375,0.02). </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Take the block that is the same colour as a traffic light that is telling cars to "go", and move it to the position (0,0.375,0.02). </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Take the block that is the colour of the Saharah Desert, and move it to the position (0,0.375,0.02). </t>
-  </si>
-  <si>
-    <t>(0.25,0.25,0.02)</t>
-  </si>
-  <si>
     <t>(-0.25,0.25,0.02)</t>
   </si>
   <si>
@@ -67,6 +52,9 @@
   </si>
   <si>
     <t>(-0.25,0.5,0.02)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Take the red block, and move it to the position (0,0.375,0.02). </t>
   </si>
 </sst>
 </file>
@@ -384,10 +372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -418,70 +406,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
         <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed task a bit
</commit_message>
<xml_diff>
--- a/data/manipulation_tasks.xlsx
+++ b/data/manipulation_tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qtcc\OneDrive\Desktop\rvl\llm_rl_for_manipulation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CDD5C49-E44D-434D-9E2C-3877B9859C54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D0EB720-B065-47F7-A9CB-C59A0B34DED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,7 +54,7 @@
     <t>(-0.25,0.5,0.02)</t>
   </si>
   <si>
-    <t xml:space="preserve">Take the red block, and move it to the position (0,0.375,0.02). </t>
+    <t xml:space="preserve">Take the red block, and move it to the position (0,0.375). </t>
   </si>
 </sst>
 </file>
@@ -375,7 +375,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>